<commit_message>
implement method 2 to 4
</commit_message>
<xml_diff>
--- a/cis.xlsx
+++ b/cis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\311766821\PycharmProjects\Python-tkinter-Project - Copy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940EA36E-438E-420A-BDBA-29FE7F02BE41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15BD97A-AC80-43A7-8286-97E16C095654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3450" yWindow="1425" windowWidth="24195" windowHeight="14775" xr2:uid="{E453006E-52BA-4E6A-AB99-9EE5C8770571}"/>
+    <workbookView xWindow="1845" yWindow="735" windowWidth="20775" windowHeight="11835" xr2:uid="{E453006E-52BA-4E6A-AB99-9EE5C8770571}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -222,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -238,12 +238,11 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -561,14 +560,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77697B56-9CA9-4D41-9337-8F1BADA10126}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C25"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.625" customWidth="1"/>
-    <col min="2" max="2" width="61" customWidth="1"/>
+    <col min="2" max="2" width="72.375" customWidth="1"/>
     <col min="3" max="3" width="25.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -590,63 +589,63 @@
       <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="7">
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="9">
+      <c r="C3" s="7">
         <v>1.2</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -657,105 +656,105 @@
       <c r="B11" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="7">
         <v>2.1</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
-      <c r="C12" s="9">
+      <c r="C12" s="7">
         <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
-      <c r="C13" s="9">
+      <c r="C13" s="7">
         <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
-      <c r="C14" s="9">
+      <c r="C14" s="7">
         <v>2.4</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
-      <c r="C15" s="9">
+      <c r="C15" s="7">
         <v>2.5</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="9">
+      <c r="C16" s="7">
         <v>2.6</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
-      <c r="C17" s="9">
+      <c r="C17" s="7">
         <v>2.7</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
-      <c r="C18" s="9">
+      <c r="C18" s="7">
         <v>2.8</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
-      <c r="C20" s="9">
+      <c r="C20" s="7">
         <v>2.12</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="7" t="s">
         <v>40</v>
       </c>
     </row>
@@ -766,98 +765,98 @@
       <c r="B26" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="7">
         <v>2.9</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
-      <c r="C27" s="6">
+      <c r="C27" s="7">
         <v>2.13</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="7" t="s">
         <v>38</v>
       </c>
       <c r="F39" s="2"/>
@@ -865,14 +864,14 @@
     <row r="40" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="7" t="s">
         <v>41</v>
       </c>
     </row>
@@ -883,7 +882,7 @@
       <c r="B42" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="7" t="s">
         <v>30</v>
       </c>
     </row>
@@ -894,7 +893,7 @@
       <c r="B43" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="7" t="s">
         <v>32</v>
       </c>
     </row>
@@ -902,7 +901,7 @@
       <c r="A44" s="5">
         <v>5</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C44" s="6" t="s">

</xml_diff>

<commit_message>
implement method 2 to 5
</commit_message>
<xml_diff>
--- a/cis.xlsx
+++ b/cis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\311766821\PycharmProjects\Python-tkinter-Project - Copy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15BD97A-AC80-43A7-8286-97E16C095654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C7DCA1-9FF4-49E7-847C-241CADD2FF46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1845" yWindow="735" windowWidth="20775" windowHeight="11835" xr2:uid="{E453006E-52BA-4E6A-AB99-9EE5C8770571}"/>
   </bookViews>
@@ -561,7 +561,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,7 +904,7 @@
       <c r="B44" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="7" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add html of 6.1 to 8.1| better UI
</commit_message>
<xml_diff>
--- a/cis.xlsx
+++ b/cis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\311766821\PycharmProjects\Python-tkinter-Project - Copy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE9F454-D320-44B7-B879-ABD9A5898423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B6EFFC-54B6-49B0-A092-0B0A5C77F0AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2535" yWindow="1425" windowWidth="20775" windowHeight="11835" xr2:uid="{E453006E-52BA-4E6A-AB99-9EE5C8770571}"/>
+    <workbookView xWindow="6645" yWindow="420" windowWidth="20775" windowHeight="11835" xr2:uid="{E453006E-52BA-4E6A-AB99-9EE5C8770571}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>شماره های مربوطه</t>
   </si>
@@ -160,6 +160,24 @@
   </si>
   <si>
     <t>8.1</t>
+  </si>
+  <si>
+    <t>نوع مخاطره</t>
+  </si>
+  <si>
+    <t>توضیحات</t>
+  </si>
+  <si>
+    <t>امن سازی با پرسمان انجام میشود.</t>
+  </si>
+  <si>
+    <t>شماره  های مربوطه</t>
+  </si>
+  <si>
+    <t>امن سازی باید بصورت دستی انجام شود و دستور SQL ندارد. (عموما مخاطرات نوع صفر)</t>
+  </si>
+  <si>
+    <t>2.10.</t>
   </si>
 </sst>
 </file>
@@ -555,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77697B56-9CA9-4D41-9337-8F1BADA10126}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,11 +584,12 @@
     <col min="1" max="1" width="12.625" customWidth="1"/>
     <col min="2" max="2" width="72.375" customWidth="1"/>
     <col min="3" max="3" width="25.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>3</v>
@@ -578,8 +597,17 @@
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8">
         <v>0</v>
       </c>
@@ -589,64 +617,94 @@
       <c r="C2" s="7">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="7">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H5">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H6">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H7">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H8">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H9">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="8">
         <v>1</v>
       </c>
@@ -657,105 +715,135 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="7">
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="7">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="7">
         <v>2.4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="7">
         <v>2.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="7">
         <v>2.6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="7">
         <v>2.7</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="7">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H19">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="7">
         <v>2.12</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H20">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H21">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H22">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H23">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H24">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H25">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="8">
         <v>2</v>
       </c>
@@ -765,92 +853,122 @@
       <c r="C26" s="7">
         <v>2.13</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H26">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="7">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H27">
+        <v>2.12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H28">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H29">
+        <v>2.14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H30">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H31">
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H32">
+        <v>2.17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H33">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H34">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H35">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="7" t="s">
@@ -858,28 +976,28 @@
       </c>
       <c r="F39" s="2"/>
     </row>
-    <row r="40" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="5">
         <v>3</v>
       </c>
@@ -890,7 +1008,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="5">
         <v>4</v>
       </c>
@@ -901,7 +1019,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="5">
         <v>5</v>
       </c>
@@ -912,7 +1030,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="24" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="5">
         <v>6</v>
       </c>

</xml_diff>